<commit_message>
Working on QR code tags
</commit_message>
<xml_diff>
--- a/KLF_Django/WebForm/ExcelDocs/MobileFoodDistro.xlsx
+++ b/KLF_Django/WebForm/ExcelDocs/MobileFoodDistro.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,70 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Breadon</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>benbreadon@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1316</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Peach Tree Lane</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>63069</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Breadon</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>benbreadon@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1316</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Peach Tree Lane</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>63069</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>